<commit_message>
i261--soft IP eit2 suite file update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/silicon_01_softip_win.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/silicon_01_softip_win.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0sngsN6DrFUqmuDZZhkIhd0EivD5xjZ0nj5fkMPZg+GIws2dGdQ895P+5SBGWtagLIQbEIRaHiBSjM2rhskk/Q==" workbookSaltValue="j22CHco5Hi8vlbKkcb9mlg==" workbookSpinCount="100000" lockStructure="1"/>
@@ -27,14 +27,14 @@
   <calcPr calcId="122211"/>
   <customWorkbookViews>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="537">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1336,9 +1336,6 @@
     <t>88</t>
   </si>
   <si>
-    <t>89</t>
-  </si>
-  <si>
     <t>Arithmetic</t>
   </si>
   <si>
@@ -1528,9 +1525,6 @@
     <t xml:space="preserve">jedi/02_Memory/09_ram_dp_true/90_ramdp_true_512x8                                                                                                         </t>
   </si>
   <si>
-    <t xml:space="preserve">jedi/02_Memory/10_lram/10_Single_Port/100_lram_sp_defualt                                                                                                 </t>
-  </si>
-  <si>
     <t xml:space="preserve">jedi/05_PMI/Memory_pmi/00_ram_dq_pmi_verilog                                                                                                              </t>
   </si>
   <si>
@@ -1781,9 +1775,6 @@
   </si>
   <si>
     <t>A_512x18    B_512x18      regA_Y rstA_syn_syn         regB_Y rstB_syn_syn    enable_byteA_n   enable_byteB_n INIT_none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP_data_32  addr_16384  write_normal      WEP_h  CEP_h   RP_h  inR_N  outR_N CP_h  PAE_n GRE_y PBE_n URE_n Ecc_n assert_sync init_none </t>
   </si>
   <si>
     <t>pmi ram_dq verilog</t>
@@ -3172,30 +3163,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="41" applyBorder="1" applyAlignment="1">
@@ -3203,9 +3210,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3222,30 +3226,17 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -5728,7 +5719,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6F5042DA-3E23-44F9-A694-62B0C11B20B0}" diskRevisions="1" revisionId="994" version="12">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{28B8FB20-C94D-4978-A2D0-B2FCBA2F1FA0}" diskRevisions="1" revisionId="1028" version="14">
   <header guid="{DB40D02A-1C38-451A-8E02-505A412F9BEE}" dateTime="2020-03-04T15:04:22" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5825,6 +5816,22 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{E2A5FE5D-38D9-4E2F-AD61-08A66134AABB}" dateTime="2020-03-10T15:24:59" maxSheetId="5" userName="Jason Wang" r:id="rId13" minRId="995" maxRId="1026">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{28B8FB20-C94D-4978-A2D0-B2FCBA2F1FA0}" dateTime="2020-03-10T15:25:03" maxSheetId="5" userName="Jason Wang" r:id="rId14">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -6484,6 +6491,455 @@
 </file>
 
 <file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="995" sId="2" ref="A60:XFD60" action="deleteRow">
+    <rfmt sheetId="2" xfDxf="1" sqref="A60:XFD60" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="30" formatCode="@"/>
+        <protection locked="0"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="A60" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="D60" t="inlineStr">
+        <is>
+          <t>Memory</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="E60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">jedi/02_Memory/10_lram/10_Single_Port/100_lram_sp_defualt                                                                                                 </t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="H60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SP_data_32  addr_16384  write_normal      WEP_h  CEP_h   RP_h  inR_N  outR_N CP_h  PAE_n GRE_y PBE_n URE_n Ecc_n assert_sync init_none </t>
+        </is>
+      </nc>
+    </rcc>
+    <rfmt sheetId="2" sqref="L60" start="0" length="0">
+      <dxf>
+        <numFmt numFmtId="0" formatCode="General"/>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="2">
+      <nc r="W60" t="inlineStr">
+        <is>
+          <t>jedi</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="2">
+      <nc r="AD60" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcc rId="996" sId="2">
+    <oc r="A60" t="inlineStr">
+      <is>
+        <t>59</t>
+      </is>
+    </oc>
+    <nc r="A60" t="inlineStr">
+      <is>
+        <t>58</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="997" sId="2">
+    <oc r="A61" t="inlineStr">
+      <is>
+        <t>60</t>
+      </is>
+    </oc>
+    <nc r="A61" t="inlineStr">
+      <is>
+        <t>59</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="998" sId="2">
+    <oc r="A62" t="inlineStr">
+      <is>
+        <t>61</t>
+      </is>
+    </oc>
+    <nc r="A62" t="inlineStr">
+      <is>
+        <t>60</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="999" sId="2">
+    <oc r="A63" t="inlineStr">
+      <is>
+        <t>62</t>
+      </is>
+    </oc>
+    <nc r="A63" t="inlineStr">
+      <is>
+        <t>61</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1000" sId="2">
+    <oc r="A64" t="inlineStr">
+      <is>
+        <t>63</t>
+      </is>
+    </oc>
+    <nc r="A64" t="inlineStr">
+      <is>
+        <t>62</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1001" sId="2">
+    <oc r="A65" t="inlineStr">
+      <is>
+        <t>64</t>
+      </is>
+    </oc>
+    <nc r="A65" t="inlineStr">
+      <is>
+        <t>63</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1002" sId="2">
+    <oc r="A66" t="inlineStr">
+      <is>
+        <t>65</t>
+      </is>
+    </oc>
+    <nc r="A66" t="inlineStr">
+      <is>
+        <t>64</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1003" sId="2">
+    <oc r="A67" t="inlineStr">
+      <is>
+        <t>66</t>
+      </is>
+    </oc>
+    <nc r="A67" t="inlineStr">
+      <is>
+        <t>65</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1004" sId="2">
+    <oc r="A68" t="inlineStr">
+      <is>
+        <t>67</t>
+      </is>
+    </oc>
+    <nc r="A68" t="inlineStr">
+      <is>
+        <t>66</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1005" sId="2">
+    <oc r="A69" t="inlineStr">
+      <is>
+        <t>68</t>
+      </is>
+    </oc>
+    <nc r="A69" t="inlineStr">
+      <is>
+        <t>67</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1006" sId="2">
+    <oc r="A70" t="inlineStr">
+      <is>
+        <t>69</t>
+      </is>
+    </oc>
+    <nc r="A70" t="inlineStr">
+      <is>
+        <t>68</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1007" sId="2">
+    <oc r="A71" t="inlineStr">
+      <is>
+        <t>70</t>
+      </is>
+    </oc>
+    <nc r="A71" t="inlineStr">
+      <is>
+        <t>69</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1008" sId="2">
+    <oc r="A72" t="inlineStr">
+      <is>
+        <t>71</t>
+      </is>
+    </oc>
+    <nc r="A72" t="inlineStr">
+      <is>
+        <t>70</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1009" sId="2">
+    <oc r="A73" t="inlineStr">
+      <is>
+        <t>72</t>
+      </is>
+    </oc>
+    <nc r="A73" t="inlineStr">
+      <is>
+        <t>71</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1010" sId="2">
+    <oc r="A74" t="inlineStr">
+      <is>
+        <t>73</t>
+      </is>
+    </oc>
+    <nc r="A74" t="inlineStr">
+      <is>
+        <t>72</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1011" sId="2">
+    <oc r="A75" t="inlineStr">
+      <is>
+        <t>74</t>
+      </is>
+    </oc>
+    <nc r="A75" t="inlineStr">
+      <is>
+        <t>73</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1012" sId="2">
+    <oc r="A76" t="inlineStr">
+      <is>
+        <t>75</t>
+      </is>
+    </oc>
+    <nc r="A76" t="inlineStr">
+      <is>
+        <t>74</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1013" sId="2">
+    <oc r="A77" t="inlineStr">
+      <is>
+        <t>76</t>
+      </is>
+    </oc>
+    <nc r="A77" t="inlineStr">
+      <is>
+        <t>75</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1014" sId="2">
+    <oc r="A78" t="inlineStr">
+      <is>
+        <t>77</t>
+      </is>
+    </oc>
+    <nc r="A78" t="inlineStr">
+      <is>
+        <t>76</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1015" sId="2">
+    <oc r="A79" t="inlineStr">
+      <is>
+        <t>78</t>
+      </is>
+    </oc>
+    <nc r="A79" t="inlineStr">
+      <is>
+        <t>77</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1016" sId="2">
+    <oc r="A80" t="inlineStr">
+      <is>
+        <t>79</t>
+      </is>
+    </oc>
+    <nc r="A80" t="inlineStr">
+      <is>
+        <t>78</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1017" sId="2">
+    <oc r="A81" t="inlineStr">
+      <is>
+        <t>80</t>
+      </is>
+    </oc>
+    <nc r="A81" t="inlineStr">
+      <is>
+        <t>79</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1018" sId="2">
+    <oc r="A82" t="inlineStr">
+      <is>
+        <t>81</t>
+      </is>
+    </oc>
+    <nc r="A82" t="inlineStr">
+      <is>
+        <t>80</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1019" sId="2">
+    <oc r="A83" t="inlineStr">
+      <is>
+        <t>82</t>
+      </is>
+    </oc>
+    <nc r="A83" t="inlineStr">
+      <is>
+        <t>81</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1020" sId="2">
+    <oc r="A84" t="inlineStr">
+      <is>
+        <t>83</t>
+      </is>
+    </oc>
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>82</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1021" sId="2">
+    <oc r="A85" t="inlineStr">
+      <is>
+        <t>84</t>
+      </is>
+    </oc>
+    <nc r="A85" t="inlineStr">
+      <is>
+        <t>83</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1022" sId="2">
+    <oc r="A86" t="inlineStr">
+      <is>
+        <t>85</t>
+      </is>
+    </oc>
+    <nc r="A86" t="inlineStr">
+      <is>
+        <t>84</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1023" sId="2">
+    <oc r="A87" t="inlineStr">
+      <is>
+        <t>86</t>
+      </is>
+    </oc>
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>85</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1024" sId="2">
+    <oc r="A88" t="inlineStr">
+      <is>
+        <t>87</t>
+      </is>
+    </oc>
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>86</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1025" sId="2">
+    <oc r="A89" t="inlineStr">
+      <is>
+        <t>88</t>
+      </is>
+    </oc>
+    <nc r="A89" t="inlineStr">
+      <is>
+        <t>87</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1026" sId="2">
+    <oc r="A90" t="inlineStr">
+      <is>
+        <t>89</t>
+      </is>
+    </oc>
+    <nc r="A90" t="inlineStr">
+      <is>
+        <t>88</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+    <oldFormula>case!$A$2:$AD$2</oldFormula>
+  </rdn>
+  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
   <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
@@ -13536,7 +13992,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -13598,13 +14054,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -13617,14 +14073,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD91"/>
+  <dimension ref="A1:AD90"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -13789,19 +14245,19 @@
         <v>272</v>
       </c>
       <c r="D3" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>360</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>361</v>
-      </c>
       <c r="H3" s="18" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="W3" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD3" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -13809,19 +14265,19 @@
         <v>273</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="W4" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD4" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -13829,19 +14285,19 @@
         <v>274</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="W5" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD5" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -13849,19 +14305,19 @@
         <v>275</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="W6" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD6" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -13869,19 +14325,19 @@
         <v>276</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="W7" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD7" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -13889,19 +14345,19 @@
         <v>277</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="W8" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD8" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -13909,19 +14365,19 @@
         <v>278</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="W9" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD9" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -13929,19 +14385,19 @@
         <v>279</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="W10" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD10" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -13949,19 +14405,19 @@
         <v>266</v>
       </c>
       <c r="D11" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>370</v>
-      </c>
       <c r="H11" s="18" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="W11" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD11" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -13969,19 +14425,19 @@
         <v>280</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="W12" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD12" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -13989,19 +14445,19 @@
         <v>281</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="W13" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD13" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -14009,19 +14465,19 @@
         <v>282</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="W14" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD14" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="15" spans="1:30">
@@ -14029,19 +14485,19 @@
         <v>283</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="W15" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD15" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -14049,19 +14505,19 @@
         <v>284</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="W16" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD16" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="17" spans="1:30">
@@ -14069,19 +14525,19 @@
         <v>285</v>
       </c>
       <c r="D17" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>377</v>
-      </c>
       <c r="H17" s="18" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="W17" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD17" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -14089,19 +14545,19 @@
         <v>286</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="W18" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD18" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -14109,19 +14565,19 @@
         <v>287</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="W19" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD19" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="20" spans="1:30">
@@ -14129,19 +14585,19 @@
         <v>288</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="W20" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD20" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="21" spans="1:30">
@@ -14149,19 +14605,19 @@
         <v>289</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="W21" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD21" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -14169,19 +14625,19 @@
         <v>290</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="W22" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD22" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -14189,19 +14645,19 @@
         <v>291</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="W23" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD23" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -14209,19 +14665,19 @@
         <v>292</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="W24" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD24" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="25" spans="1:30">
@@ -14229,19 +14685,19 @@
         <v>293</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="W25" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD25" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="26" spans="1:30">
@@ -14249,19 +14705,19 @@
         <v>294</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="W26" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD26" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="27" spans="1:30">
@@ -14269,19 +14725,19 @@
         <v>295</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="W27" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD27" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="28" spans="1:30">
@@ -14289,19 +14745,19 @@
         <v>296</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="W28" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD28" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="29" spans="1:30">
@@ -14309,19 +14765,19 @@
         <v>297</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="W29" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD29" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="30" spans="1:30">
@@ -14329,19 +14785,19 @@
         <v>298</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="W30" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD30" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="31" spans="1:30">
@@ -14349,19 +14805,19 @@
         <v>299</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="W31" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD31" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="32" spans="1:30">
@@ -14369,19 +14825,19 @@
         <v>300</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="W32" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD32" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="33" spans="1:30">
@@ -14389,19 +14845,19 @@
         <v>301</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="W33" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD33" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="34" spans="1:30">
@@ -14409,19 +14865,19 @@
         <v>302</v>
       </c>
       <c r="D34" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>394</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>395</v>
-      </c>
       <c r="H34" s="18" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="W34" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD34" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="35" spans="1:30">
@@ -14429,19 +14885,19 @@
         <v>303</v>
       </c>
       <c r="D35" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="E35" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>397</v>
-      </c>
       <c r="H35" s="18" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="W35" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD35" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="36" spans="1:30">
@@ -14449,19 +14905,19 @@
         <v>304</v>
       </c>
       <c r="D36" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="E36" s="18" t="s">
         <v>398</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>399</v>
-      </c>
       <c r="H36" s="18" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="W36" s="18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AD36" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="37" spans="1:30">
@@ -14469,19 +14925,19 @@
         <v>305</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="W37" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD37" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="38" spans="1:30">
@@ -14489,19 +14945,19 @@
         <v>306</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="W38" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD38" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="39" spans="1:30">
@@ -14509,19 +14965,19 @@
         <v>307</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="W39" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD39" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="40" spans="1:30">
@@ -14529,19 +14985,19 @@
         <v>308</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="W40" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD40" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="41" spans="1:30">
@@ -14549,19 +15005,19 @@
         <v>309</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="W41" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD41" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -14569,19 +15025,19 @@
         <v>310</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="W42" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD42" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="43" spans="1:30">
@@ -14589,19 +15045,19 @@
         <v>311</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="W43" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD43" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="44" spans="1:30">
@@ -14609,19 +15065,19 @@
         <v>312</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="W44" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD44" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="45" spans="1:30">
@@ -14629,19 +15085,19 @@
         <v>313</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="W45" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD45" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="46" spans="1:30">
@@ -14649,19 +15105,19 @@
         <v>314</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="W46" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD46" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="47" spans="1:30">
@@ -14669,19 +15125,19 @@
         <v>315</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="W47" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD47" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="48" spans="1:30">
@@ -14689,19 +15145,19 @@
         <v>316</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="W48" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD48" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="49" spans="1:30">
@@ -14709,19 +15165,19 @@
         <v>317</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="W49" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD49" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="50" spans="1:30">
@@ -14729,19 +15185,19 @@
         <v>318</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="W50" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD50" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="51" spans="1:30">
@@ -14749,19 +15205,19 @@
         <v>319</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="W51" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD51" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="52" spans="1:30">
@@ -14769,19 +15225,19 @@
         <v>320</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="W52" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD52" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="53" spans="1:30">
@@ -14789,19 +15245,19 @@
         <v>321</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="W53" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD53" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="54" spans="1:30">
@@ -14809,19 +15265,19 @@
         <v>322</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="W54" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD54" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="55" spans="1:30">
@@ -14829,19 +15285,19 @@
         <v>323</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="W55" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD55" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="56" spans="1:30">
@@ -14849,19 +15305,19 @@
         <v>324</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="W56" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD56" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="57" spans="1:30">
@@ -14869,19 +15325,19 @@
         <v>325</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="W57" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD57" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="58" spans="1:30">
@@ -14889,19 +15345,19 @@
         <v>326</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="W58" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD58" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="59" spans="1:30">
@@ -14909,19 +15365,19 @@
         <v>327</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="W59" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD59" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="60" spans="1:30">
@@ -14929,19 +15385,19 @@
         <v>328</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="W60" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD60" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="61" spans="1:30">
@@ -14949,19 +15405,19 @@
         <v>329</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="W61" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD61" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="62" spans="1:30">
@@ -14969,19 +15425,19 @@
         <v>330</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="W62" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD62" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="63" spans="1:30">
@@ -14989,19 +15445,19 @@
         <v>331</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="W63" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD63" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="64" spans="1:30">
@@ -15009,19 +15465,19 @@
         <v>332</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="W64" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD64" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="65" spans="1:30">
@@ -15029,19 +15485,19 @@
         <v>333</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="W65" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD65" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="66" spans="1:30">
@@ -15049,19 +15505,19 @@
         <v>334</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="W66" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD66" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="67" spans="1:30">
@@ -15069,19 +15525,19 @@
         <v>335</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="W67" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD67" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="68" spans="1:30">
@@ -15089,19 +15545,19 @@
         <v>336</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="W68" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD68" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="69" spans="1:30">
@@ -15109,19 +15565,19 @@
         <v>337</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E69" s="18" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="W69" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD69" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="70" spans="1:30">
@@ -15129,19 +15585,19 @@
         <v>338</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="W70" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD70" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="71" spans="1:30">
@@ -15149,19 +15605,19 @@
         <v>339</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="W71" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD71" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="72" spans="1:30">
@@ -15169,19 +15625,19 @@
         <v>340</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="W72" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD72" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="73" spans="1:30">
@@ -15189,19 +15645,19 @@
         <v>341</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="W73" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD73" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="74" spans="1:30">
@@ -15209,19 +15665,19 @@
         <v>342</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E74" s="18" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H74" s="18" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="W74" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD74" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="75" spans="1:30">
@@ -15229,19 +15685,19 @@
         <v>343</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="W75" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD75" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="76" spans="1:30">
@@ -15249,19 +15705,19 @@
         <v>344</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="W76" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD76" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="77" spans="1:30">
@@ -15269,19 +15725,19 @@
         <v>345</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H77" s="18" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="W77" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD77" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="78" spans="1:30">
@@ -15289,19 +15745,16 @@
         <v>346</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>376</v>
+        <v>440</v>
       </c>
       <c r="E78" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="H78" s="18" t="s">
-        <v>526</v>
-      </c>
       <c r="W78" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD78" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="79" spans="1:30">
@@ -15309,16 +15762,19 @@
         <v>347</v>
       </c>
       <c r="D79" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="E79" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="E79" s="18" t="s">
-        <v>443</v>
+      <c r="H79" s="18" t="s">
+        <v>524</v>
       </c>
       <c r="W79" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD79" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="80" spans="1:30">
@@ -15326,19 +15782,19 @@
         <v>348</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H80" s="18" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="W80" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD80" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="81" spans="1:30">
@@ -15346,19 +15802,19 @@
         <v>349</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E81" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H81" s="18" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="W81" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD81" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="82" spans="1:30">
@@ -15366,19 +15822,19 @@
         <v>350</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H82" s="18" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="W82" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD82" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="83" spans="1:30">
@@ -15386,19 +15842,19 @@
         <v>351</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="W83" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD83" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="84" spans="1:30">
@@ -15406,19 +15862,19 @@
         <v>352</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H84" s="18" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="W84" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD84" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="85" spans="1:30">
@@ -15426,19 +15882,16 @@
         <v>353</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="E85" s="18" t="s">
         <v>449</v>
       </c>
-      <c r="H85" s="18" t="s">
-        <v>532</v>
-      </c>
       <c r="W85" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD85" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="86" spans="1:30">
@@ -15446,16 +15899,16 @@
         <v>354</v>
       </c>
       <c r="D86" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="E86" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="E86" s="18" t="s">
-        <v>451</v>
-      </c>
       <c r="W86" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD86" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="87" spans="1:30">
@@ -15463,16 +15916,16 @@
         <v>355</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E87" s="18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="W87" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD87" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="88" spans="1:30">
@@ -15480,16 +15933,19 @@
         <v>356</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>453</v>
+        <v>452</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>530</v>
       </c>
       <c r="W88" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD88" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="89" spans="1:30">
@@ -15497,19 +15953,19 @@
         <v>357</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H89" s="18" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="W89" s="18" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD89" s="18" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="90" spans="1:30">
@@ -15517,62 +15973,42 @@
         <v>358</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E90" s="18" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H90" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="W90" s="18" t="s">
         <v>534</v>
       </c>
-      <c r="W90" s="18" t="s">
-        <v>537</v>
-      </c>
       <c r="AD90" s="18" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="91" spans="1:30">
-      <c r="A91" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="D91" s="18" t="s">
-        <v>450</v>
-      </c>
-      <c r="E91" s="18" t="s">
-        <v>456</v>
-      </c>
-      <c r="H91" s="18" t="s">
         <v>535</v>
-      </c>
-      <c r="W91" s="18" t="s">
-        <v>537</v>
-      </c>
-      <c r="AD91" s="18" t="s">
-        <v>538</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="4C55417S7/WEfM6p9p+2qxLa3pFuuwTQvkVS+xLflxPJ6JUMhmXb8UBi2EhWPKsWHpV7wPPZoM4Ci73L5pzjfA==" saltValue="OVPlytvnGy6tQU/SUgOtyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="55" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="70" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B90" sqref="B90"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A2:AD2"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:Y2"/>
@@ -15588,7 +16024,7 @@
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:V1 A1:I1">
-      <formula1>$F$119:$J$119</formula1>
+      <formula1>$F$118:$J$118</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15716,17 +16152,17 @@
       <c r="E109" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F109" s="93" t="s">
+      <c r="F109" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G109" s="94"/>
-      <c r="H109" s="94"/>
-      <c r="I109" s="94"/>
-      <c r="J109" s="94"/>
-      <c r="K109" s="94"/>
-      <c r="L109" s="94"/>
-      <c r="M109" s="94"/>
-      <c r="N109" s="95"/>
+      <c r="G109" s="74"/>
+      <c r="H109" s="74"/>
+      <c r="I109" s="74"/>
+      <c r="J109" s="74"/>
+      <c r="K109" s="74"/>
+      <c r="L109" s="74"/>
+      <c r="M109" s="74"/>
+      <c r="N109" s="75"/>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="6" t="s">
@@ -16564,7 +17000,7 @@
       <c r="A144" s="41">
         <v>1</v>
       </c>
-      <c r="B144" s="96" t="s">
+      <c r="B144" s="76" t="s">
         <v>122</v>
       </c>
       <c r="C144" s="39" t="s">
@@ -16590,7 +17026,7 @@
       <c r="A145" s="41">
         <v>2</v>
       </c>
-      <c r="B145" s="97"/>
+      <c r="B145" s="77"/>
       <c r="C145" s="39" t="s">
         <v>128</v>
       </c>
@@ -16612,7 +17048,7 @@
       <c r="A146" s="59">
         <v>3</v>
       </c>
-      <c r="B146" s="97"/>
+      <c r="B146" s="77"/>
       <c r="C146" s="39" t="s">
         <v>9</v>
       </c>
@@ -16630,7 +17066,7 @@
       <c r="A147" s="59">
         <v>4</v>
       </c>
-      <c r="B147" s="97"/>
+      <c r="B147" s="77"/>
       <c r="C147" s="60" t="s">
         <v>256</v>
       </c>
@@ -16652,7 +17088,7 @@
       <c r="A148" s="59">
         <v>5</v>
       </c>
-      <c r="B148" s="97"/>
+      <c r="B148" s="77"/>
       <c r="C148" s="39" t="s">
         <v>253</v>
       </c>
@@ -16672,7 +17108,7 @@
       <c r="A149" s="59">
         <v>6</v>
       </c>
-      <c r="B149" s="97"/>
+      <c r="B149" s="77"/>
       <c r="C149" s="60" t="s">
         <v>254</v>
       </c>
@@ -16694,7 +17130,7 @@
       <c r="A150" s="59">
         <v>7</v>
       </c>
-      <c r="B150" s="97"/>
+      <c r="B150" s="77"/>
       <c r="C150" s="39" t="s">
         <v>130</v>
       </c>
@@ -16716,7 +17152,7 @@
       <c r="A151" s="59">
         <v>8</v>
       </c>
-      <c r="B151" s="97"/>
+      <c r="B151" s="77"/>
       <c r="C151" s="39" t="s">
         <v>246</v>
       </c>
@@ -16738,7 +17174,7 @@
       <c r="A152" s="59">
         <v>9</v>
       </c>
-      <c r="B152" s="97"/>
+      <c r="B152" s="77"/>
       <c r="C152" s="39" t="s">
         <v>55</v>
       </c>
@@ -16762,7 +17198,7 @@
       <c r="A153" s="59">
         <v>10</v>
       </c>
-      <c r="B153" s="83"/>
+      <c r="B153" s="78"/>
       <c r="C153" s="39" t="s">
         <v>136</v>
       </c>
@@ -16784,7 +17220,7 @@
       <c r="A154" s="59">
         <v>11</v>
       </c>
-      <c r="B154" s="79" t="s">
+      <c r="B154" s="72" t="s">
         <v>139</v>
       </c>
       <c r="C154" s="39" t="s">
@@ -16810,7 +17246,7 @@
       <c r="A155" s="59">
         <v>12</v>
       </c>
-      <c r="B155" s="79"/>
+      <c r="B155" s="72"/>
       <c r="C155" s="39" t="s">
         <v>247</v>
       </c>
@@ -16834,7 +17270,7 @@
       <c r="A156" s="59">
         <v>13</v>
       </c>
-      <c r="B156" s="96" t="s">
+      <c r="B156" s="76" t="s">
         <v>143</v>
       </c>
       <c r="C156" s="39" t="s">
@@ -16858,7 +17294,7 @@
       <c r="A157" s="59">
         <v>14</v>
       </c>
-      <c r="B157" s="83"/>
+      <c r="B157" s="78"/>
       <c r="C157" s="39" t="s">
         <v>146</v>
       </c>
@@ -16878,7 +17314,7 @@
       <c r="A158" s="59">
         <v>15</v>
       </c>
-      <c r="B158" s="79" t="s">
+      <c r="B158" s="72" t="s">
         <v>148</v>
       </c>
       <c r="C158" s="39" t="s">
@@ -16902,7 +17338,7 @@
       <c r="A159" s="59">
         <v>16</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="72"/>
       <c r="C159" s="39" t="s">
         <v>152</v>
       </c>
@@ -16922,7 +17358,7 @@
       <c r="A160" s="59">
         <v>17</v>
       </c>
-      <c r="B160" s="79"/>
+      <c r="B160" s="72"/>
       <c r="C160" s="39" t="s">
         <v>153</v>
       </c>
@@ -16942,7 +17378,7 @@
       <c r="A161" s="59">
         <v>18</v>
       </c>
-      <c r="B161" s="79"/>
+      <c r="B161" s="72"/>
       <c r="C161" s="39" t="s">
         <v>154</v>
       </c>
@@ -16962,7 +17398,7 @@
       <c r="A162" s="59">
         <v>19</v>
       </c>
-      <c r="B162" s="79"/>
+      <c r="B162" s="72"/>
       <c r="C162" s="39" t="s">
         <v>155</v>
       </c>
@@ -16982,7 +17418,7 @@
       <c r="A163" s="59">
         <v>20</v>
       </c>
-      <c r="B163" s="79"/>
+      <c r="B163" s="72"/>
       <c r="C163" s="39" t="s">
         <v>156</v>
       </c>
@@ -17002,7 +17438,7 @@
       <c r="A164" s="59">
         <v>21</v>
       </c>
-      <c r="B164" s="79"/>
+      <c r="B164" s="72"/>
       <c r="C164" s="39" t="s">
         <v>157</v>
       </c>
@@ -17022,7 +17458,7 @@
       <c r="A165" s="59">
         <v>22</v>
       </c>
-      <c r="B165" s="79"/>
+      <c r="B165" s="72"/>
       <c r="C165" s="39" t="s">
         <v>158</v>
       </c>
@@ -17042,7 +17478,7 @@
       <c r="A166" s="59">
         <v>23</v>
       </c>
-      <c r="B166" s="79" t="s">
+      <c r="B166" s="72" t="s">
         <v>159</v>
       </c>
       <c r="C166" s="39" t="s">
@@ -17066,7 +17502,7 @@
       <c r="A167" s="59">
         <v>24</v>
       </c>
-      <c r="B167" s="79"/>
+      <c r="B167" s="72"/>
       <c r="C167" s="39" t="s">
         <v>163</v>
       </c>
@@ -17088,7 +17524,7 @@
       <c r="A168" s="59">
         <v>25</v>
       </c>
-      <c r="B168" s="79"/>
+      <c r="B168" s="72"/>
       <c r="C168" s="39" t="s">
         <v>166</v>
       </c>
@@ -17110,7 +17546,7 @@
       <c r="A169" s="59">
         <v>26</v>
       </c>
-      <c r="B169" s="79" t="s">
+      <c r="B169" s="72" t="s">
         <v>169</v>
       </c>
       <c r="C169" s="39" t="s">
@@ -17134,7 +17570,7 @@
       <c r="A170" s="59">
         <v>27</v>
       </c>
-      <c r="B170" s="79"/>
+      <c r="B170" s="72"/>
       <c r="C170" s="39" t="s">
         <v>172</v>
       </c>
@@ -17156,7 +17592,7 @@
       <c r="A171" s="42">
         <v>28</v>
       </c>
-      <c r="B171" s="80"/>
+      <c r="B171" s="79"/>
       <c r="C171" s="40"/>
       <c r="D171" s="40"/>
       <c r="E171" s="40"/>
@@ -17192,11 +17628,11 @@
       <c r="B185" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="C185" s="89" t="s">
+      <c r="C185" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D185" s="89"/>
-      <c r="E185" s="89"/>
+      <c r="D185" s="80"/>
+      <c r="E185" s="80"/>
       <c r="F185" s="34" t="s">
         <v>42</v>
       </c>
@@ -17205,17 +17641,17 @@
       </c>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="79" t="s">
+      <c r="A186" s="72" t="s">
         <v>180</v>
       </c>
-      <c r="B186" s="79" t="s">
+      <c r="B186" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="90" t="s">
+      <c r="C186" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="D186" s="90"/>
-      <c r="E186" s="90"/>
+      <c r="D186" s="81"/>
+      <c r="E186" s="81"/>
       <c r="F186" s="39" t="s">
         <v>183</v>
       </c>
@@ -17224,13 +17660,13 @@
       </c>
     </row>
     <row r="187" spans="1:7">
-      <c r="A187" s="79"/>
-      <c r="B187" s="79"/>
-      <c r="C187" s="91" t="s">
+      <c r="A187" s="72"/>
+      <c r="B187" s="72"/>
+      <c r="C187" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="D187" s="91"/>
-      <c r="E187" s="91"/>
+      <c r="D187" s="82"/>
+      <c r="E187" s="82"/>
       <c r="F187" s="39" t="s">
         <v>185</v>
       </c>
@@ -17239,15 +17675,15 @@
       </c>
     </row>
     <row r="188" spans="1:7">
-      <c r="A188" s="79"/>
-      <c r="B188" s="79" t="s">
+      <c r="A188" s="72"/>
+      <c r="B188" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="92" t="s">
+      <c r="C188" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="D188" s="92"/>
-      <c r="E188" s="92"/>
+      <c r="D188" s="83"/>
+      <c r="E188" s="83"/>
       <c r="F188" s="39" t="s">
         <v>183</v>
       </c>
@@ -17256,13 +17692,13 @@
       </c>
     </row>
     <row r="189" spans="1:7">
-      <c r="A189" s="79"/>
-      <c r="B189" s="79"/>
-      <c r="C189" s="92" t="s">
+      <c r="A189" s="72"/>
+      <c r="B189" s="72"/>
+      <c r="C189" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="D189" s="92"/>
-      <c r="E189" s="92"/>
+      <c r="D189" s="83"/>
+      <c r="E189" s="83"/>
       <c r="F189" s="39" t="s">
         <v>185</v>
       </c>
@@ -17271,17 +17707,17 @@
       </c>
     </row>
     <row r="190" spans="1:7">
-      <c r="A190" s="77" t="s">
+      <c r="A190" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="B190" s="79" t="s">
+      <c r="B190" s="72" t="s">
         <v>189</v>
       </c>
-      <c r="C190" s="79" t="s">
+      <c r="C190" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="D190" s="79"/>
-      <c r="E190" s="79"/>
+      <c r="D190" s="72"/>
+      <c r="E190" s="72"/>
       <c r="F190" s="39" t="s">
         <v>183</v>
       </c>
@@ -17290,13 +17726,13 @@
       </c>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="77"/>
-      <c r="B191" s="79"/>
-      <c r="C191" s="79" t="s">
+      <c r="A191" s="84"/>
+      <c r="B191" s="72"/>
+      <c r="C191" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="D191" s="79"/>
-      <c r="E191" s="79"/>
+      <c r="D191" s="72"/>
+      <c r="E191" s="72"/>
       <c r="F191" s="39" t="s">
         <v>185</v>
       </c>
@@ -17305,15 +17741,15 @@
       </c>
     </row>
     <row r="192" spans="1:7">
-      <c r="A192" s="77"/>
-      <c r="B192" s="79" t="s">
+      <c r="A192" s="84"/>
+      <c r="B192" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="79" t="s">
+      <c r="C192" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="D192" s="79"/>
-      <c r="E192" s="79"/>
+      <c r="D192" s="72"/>
+      <c r="E192" s="72"/>
       <c r="F192" s="39" t="s">
         <v>183</v>
       </c>
@@ -17322,13 +17758,13 @@
       </c>
     </row>
     <row r="193" spans="1:7">
-      <c r="A193" s="77"/>
-      <c r="B193" s="79"/>
-      <c r="C193" s="79" t="s">
+      <c r="A193" s="84"/>
+      <c r="B193" s="72"/>
+      <c r="C193" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="D193" s="79"/>
-      <c r="E193" s="79"/>
+      <c r="D193" s="72"/>
+      <c r="E193" s="72"/>
       <c r="F193" s="39" t="s">
         <v>185</v>
       </c>
@@ -17337,17 +17773,17 @@
       </c>
     </row>
     <row r="194" spans="1:7">
-      <c r="A194" s="77" t="s">
+      <c r="A194" s="84" t="s">
         <v>191</v>
       </c>
-      <c r="B194" s="79" t="s">
+      <c r="B194" s="72" t="s">
         <v>192</v>
       </c>
-      <c r="C194" s="79" t="s">
+      <c r="C194" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="D194" s="79"/>
-      <c r="E194" s="79"/>
+      <c r="D194" s="72"/>
+      <c r="E194" s="72"/>
       <c r="F194" s="39" t="s">
         <v>183</v>
       </c>
@@ -17356,13 +17792,13 @@
       </c>
     </row>
     <row r="195" spans="1:7">
-      <c r="A195" s="77"/>
-      <c r="B195" s="79"/>
-      <c r="C195" s="79" t="s">
+      <c r="A195" s="84"/>
+      <c r="B195" s="72"/>
+      <c r="C195" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="D195" s="79"/>
-      <c r="E195" s="79"/>
+      <c r="D195" s="72"/>
+      <c r="E195" s="72"/>
       <c r="F195" s="39" t="s">
         <v>185</v>
       </c>
@@ -17371,15 +17807,15 @@
       </c>
     </row>
     <row r="196" spans="1:7">
-      <c r="A196" s="77"/>
-      <c r="B196" s="79" t="s">
+      <c r="A196" s="84"/>
+      <c r="B196" s="72" t="s">
         <v>193</v>
       </c>
-      <c r="C196" s="79" t="s">
+      <c r="C196" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="D196" s="79"/>
-      <c r="E196" s="79"/>
+      <c r="D196" s="72"/>
+      <c r="E196" s="72"/>
       <c r="F196" s="39" t="s">
         <v>183</v>
       </c>
@@ -17388,13 +17824,13 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A197" s="78"/>
-      <c r="B197" s="80"/>
-      <c r="C197" s="80" t="s">
+      <c r="A197" s="86"/>
+      <c r="B197" s="79"/>
+      <c r="C197" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="D197" s="80"/>
-      <c r="E197" s="80"/>
+      <c r="D197" s="79"/>
+      <c r="E197" s="79"/>
       <c r="F197" s="40" t="s">
         <v>185</v>
       </c>
@@ -17433,12 +17869,12 @@
       <c r="A202" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B202" s="81" t="s">
+      <c r="B202" s="87" t="s">
         <v>198</v>
       </c>
-      <c r="C202" s="81"/>
-      <c r="D202" s="81"/>
-      <c r="E202" s="81"/>
+      <c r="C202" s="87"/>
+      <c r="D202" s="87"/>
+      <c r="E202" s="87"/>
       <c r="F202" s="22" t="s">
         <v>199</v>
       </c>
@@ -17450,12 +17886,12 @@
       <c r="A203" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B203" s="82" t="s">
+      <c r="B203" s="88" t="s">
         <v>202</v>
       </c>
-      <c r="C203" s="83"/>
-      <c r="D203" s="83"/>
-      <c r="E203" s="83"/>
+      <c r="C203" s="78"/>
+      <c r="D203" s="78"/>
+      <c r="E203" s="78"/>
       <c r="F203" s="36" t="s">
         <v>203</v>
       </c>
@@ -17467,12 +17903,12 @@
       <c r="A204" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="84" t="s">
+      <c r="B204" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="C204" s="85"/>
-      <c r="D204" s="85"/>
-      <c r="E204" s="86"/>
+      <c r="C204" s="90"/>
+      <c r="D204" s="90"/>
+      <c r="E204" s="91"/>
       <c r="F204" s="10" t="s">
         <v>184</v>
       </c>
@@ -17484,12 +17920,12 @@
       <c r="A205" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="B205" s="84" t="s">
+      <c r="B205" s="89" t="s">
         <v>233</v>
       </c>
-      <c r="C205" s="85"/>
-      <c r="D205" s="85"/>
-      <c r="E205" s="86"/>
+      <c r="C205" s="90"/>
+      <c r="D205" s="90"/>
+      <c r="E205" s="91"/>
       <c r="F205" s="46" t="s">
         <v>231</v>
       </c>
@@ -17501,12 +17937,12 @@
       <c r="A206" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B206" s="87" t="s">
+      <c r="B206" s="92" t="s">
         <v>234</v>
       </c>
-      <c r="C206" s="80"/>
-      <c r="D206" s="80"/>
-      <c r="E206" s="80"/>
+      <c r="C206" s="79"/>
+      <c r="D206" s="79"/>
+      <c r="E206" s="79"/>
       <c r="F206" s="13" t="s">
         <v>184</v>
       </c>
@@ -17551,11 +17987,11 @@
       <c r="C211" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D211" s="88" t="s">
+      <c r="D211" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="E211" s="88"/>
-      <c r="F211" s="88"/>
+      <c r="E211" s="93"/>
+      <c r="F211" s="93"/>
       <c r="G211" s="32"/>
     </row>
     <row r="212" spans="1:7">
@@ -17568,11 +18004,11 @@
       <c r="C212" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="72" t="s">
+      <c r="D212" s="85" t="s">
         <v>54</v>
       </c>
-      <c r="E212" s="72"/>
-      <c r="F212" s="72"/>
+      <c r="E212" s="85"/>
+      <c r="F212" s="85"/>
       <c r="G212" s="24"/>
     </row>
     <row r="213" spans="1:7">
@@ -17585,11 +18021,11 @@
       <c r="C213" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="72" t="s">
+      <c r="D213" s="85" t="s">
         <v>209</v>
       </c>
-      <c r="E213" s="72"/>
-      <c r="F213" s="72"/>
+      <c r="E213" s="85"/>
+      <c r="F213" s="85"/>
       <c r="G213" s="24"/>
     </row>
     <row r="214" spans="1:7">
@@ -17602,11 +18038,11 @@
       <c r="C214" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="D214" s="72" t="s">
+      <c r="D214" s="85" t="s">
         <v>211</v>
       </c>
-      <c r="E214" s="72"/>
-      <c r="F214" s="72"/>
+      <c r="E214" s="85"/>
+      <c r="F214" s="85"/>
       <c r="G214" s="24"/>
     </row>
     <row r="215" spans="1:7">
@@ -17619,11 +18055,11 @@
       <c r="C215" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D215" s="72" t="s">
+      <c r="D215" s="85" t="s">
         <v>222</v>
       </c>
-      <c r="E215" s="72"/>
-      <c r="F215" s="72"/>
+      <c r="E215" s="85"/>
+      <c r="F215" s="85"/>
       <c r="G215" s="24"/>
     </row>
     <row r="216" spans="1:7">
@@ -17636,11 +18072,11 @@
       <c r="C216" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="D216" s="72" t="s">
+      <c r="D216" s="85" t="s">
         <v>235</v>
       </c>
-      <c r="E216" s="72"/>
-      <c r="F216" s="72"/>
+      <c r="E216" s="85"/>
+      <c r="F216" s="85"/>
       <c r="G216" s="24"/>
     </row>
     <row r="217" spans="1:7">
@@ -17653,11 +18089,11 @@
       <c r="C217" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D217" s="74" t="s">
+      <c r="D217" s="95" t="s">
         <v>237</v>
       </c>
-      <c r="E217" s="75"/>
-      <c r="F217" s="76"/>
+      <c r="E217" s="96"/>
+      <c r="F217" s="97"/>
       <c r="G217" s="53"/>
     </row>
     <row r="218" spans="1:7">
@@ -17670,11 +18106,11 @@
       <c r="C218" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="D218" s="74" t="s">
+      <c r="D218" s="95" t="s">
         <v>238</v>
       </c>
-      <c r="E218" s="75"/>
-      <c r="F218" s="76"/>
+      <c r="E218" s="96"/>
+      <c r="F218" s="97"/>
       <c r="G218" s="53"/>
     </row>
     <row r="219" spans="1:7">
@@ -17687,11 +18123,11 @@
       <c r="C219" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D219" s="74" t="s">
+      <c r="D219" s="95" t="s">
         <v>251</v>
       </c>
-      <c r="E219" s="75"/>
-      <c r="F219" s="76"/>
+      <c r="E219" s="96"/>
+      <c r="F219" s="97"/>
       <c r="G219" s="53"/>
     </row>
     <row r="220" spans="1:7">
@@ -17738,11 +18174,11 @@
       <c r="C222" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D222" s="73" t="s">
+      <c r="D222" s="94" t="s">
         <v>264</v>
       </c>
-      <c r="E222" s="73"/>
-      <c r="F222" s="73"/>
+      <c r="E222" s="94"/>
+      <c r="F222" s="94"/>
       <c r="G222" s="25"/>
     </row>
   </sheetData>
@@ -17755,28 +18191,14 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="44">
-    <mergeCell ref="B166:B168"/>
-    <mergeCell ref="F109:N109"/>
-    <mergeCell ref="B144:B153"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="B158:B165"/>
-    <mergeCell ref="B169:B171"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="A190:A193"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="D214:F214"/>
+    <mergeCell ref="D215:F215"/>
+    <mergeCell ref="D216:F216"/>
+    <mergeCell ref="D222:F222"/>
+    <mergeCell ref="D217:F217"/>
+    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="D219:F219"/>
     <mergeCell ref="D212:F212"/>
     <mergeCell ref="A194:A197"/>
     <mergeCell ref="B194:B195"/>
@@ -17791,14 +18213,28 @@
     <mergeCell ref="B206:E206"/>
     <mergeCell ref="D211:F211"/>
     <mergeCell ref="B205:E205"/>
-    <mergeCell ref="D213:F213"/>
-    <mergeCell ref="D214:F214"/>
-    <mergeCell ref="D215:F215"/>
-    <mergeCell ref="D216:F216"/>
-    <mergeCell ref="D222:F222"/>
-    <mergeCell ref="D217:F217"/>
-    <mergeCell ref="D218:F218"/>
-    <mergeCell ref="D219:F219"/>
+    <mergeCell ref="A190:A193"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="B169:B171"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="B166:B168"/>
+    <mergeCell ref="F109:N109"/>
+    <mergeCell ref="B144:B153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="B158:B165"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17825,11 +18261,11 @@
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>